<commit_message>
added new data files for figures
</commit_message>
<xml_diff>
--- a/4_aviation/net_zero_scenarios/data/data.xlsx
+++ b/4_aviation/net_zero_scenarios/data/data.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelweinold/github/phd_publication_figures/4_aviation/net_zero_scenarios/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E25855B-EC5B-2E42-8822-2FA48EF68DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF80800F-8BF4-AA45-9731-6F2C9D45DAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{A6288964-F0E9-F642-9207-3337EEFED402}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{A6288964-F0E9-F642-9207-3337EEFED402}"/>
   </bookViews>
   <sheets>
-    <sheet name="Swiss" sheetId="3" r:id="rId1"/>
+    <sheet name="Eurocontrol" sheetId="4" r:id="rId1"/>
+    <sheet name="WayPoint2050" sheetId="5" r:id="rId2"/>
+    <sheet name="Swiss" sheetId="3" r:id="rId3"/>
+    <sheet name="Destination2050" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="wpd_datasets_2" localSheetId="0">Swiss!$A$1:$N$24</definedName>
+    <definedName name="wpd_datasets_2" localSheetId="2">Swiss!$A$1:$N$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
   <si>
     <t>reduced_x</t>
   </si>
@@ -106,6 +109,54 @@
   </si>
   <si>
     <t>history_y</t>
+  </si>
+  <si>
+    <t>Other (x)</t>
+  </si>
+  <si>
+    <t>Other (y)</t>
+  </si>
+  <si>
+    <t>SAF (x)</t>
+  </si>
+  <si>
+    <t>SAF (y)</t>
+  </si>
+  <si>
+    <t>ATM (x)</t>
+  </si>
+  <si>
+    <t>ATM (y)</t>
+  </si>
+  <si>
+    <t>Fleet revol (x)</t>
+  </si>
+  <si>
+    <t>Fleet revol (y)</t>
+  </si>
+  <si>
+    <t>Fleet evol (x)</t>
+  </si>
+  <si>
+    <t>Fleet evol (y)</t>
+  </si>
+  <si>
+    <t>Market-Based Measure (x)</t>
+  </si>
+  <si>
+    <t>Market-Based Measure (y)</t>
+  </si>
+  <si>
+    <t>Operations and Infrastructure (x)</t>
+  </si>
+  <si>
+    <t>Operations and Infrastructure (y)</t>
+  </si>
+  <si>
+    <t>Technology (x)</t>
+  </si>
+  <si>
+    <t>Technology (y)</t>
   </si>
 </sst>
 </file>
@@ -460,11 +511,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885E7847-E21B-384A-B3EE-239A97221160}">
+  <dimension ref="A1:J1"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60248756-7A13-B544-A066-4CFE938C0EA1}">
+  <dimension ref="A1:H1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8018BEA-49B9-1B42-9A7A-5348ADC7F270}">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" workbookViewId="0">
-      <selection activeCell="D27" sqref="D26:D27"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,4 +1058,16 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C5AF1E-8720-AD4D-AE69-58E15F872AB8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added figure and data
</commit_message>
<xml_diff>
--- a/4_aviation/net_zero_scenarios/data/data.xlsx
+++ b/4_aviation/net_zero_scenarios/data/data.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelweinold/github/phd_publication_figures/4_aviation/net_zero_scenarios/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91E18A69-AA4B-BD4D-B858-0BEE835E8B98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBE07B7-E5AC-FA4D-A86E-229EDEBBDD2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="1" xr2:uid="{A6288964-F0E9-F642-9207-3337EEFED402}"/>
+    <workbookView xWindow="-76800" yWindow="-15380" windowWidth="25600" windowHeight="28300" activeTab="2" xr2:uid="{A6288964-F0E9-F642-9207-3337EEFED402}"/>
   </bookViews>
   <sheets>
     <sheet name="Eurocontrol" sheetId="4" r:id="rId1"/>
     <sheet name="WayPoint2050" sheetId="5" r:id="rId2"/>
-    <sheet name="Swiss" sheetId="3" r:id="rId3"/>
-    <sheet name="Destination2050" sheetId="6" r:id="rId4"/>
+    <sheet name="CORSIA" sheetId="7" r:id="rId3"/>
+    <sheet name="Swiss" sheetId="3" r:id="rId4"/>
+    <sheet name="Destination2050" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="wpd_datasets_2" localSheetId="2">Swiss!$A$1:$N$24</definedName>
+    <definedName name="wpd_datasets_2" localSheetId="3">Swiss!$A$1:$N$24</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -67,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="680">
   <si>
     <t>Other (x)</t>
   </si>
@@ -2083,6 +2084,30 @@
   </si>
   <si>
     <t xml:space="preserve"> 5,972185394295596</t>
+  </si>
+  <si>
+    <t>net (x)</t>
+  </si>
+  <si>
+    <t>net (y)</t>
+  </si>
+  <si>
+    <t>tech (x)</t>
+  </si>
+  <si>
+    <t>tech (y)</t>
+  </si>
+  <si>
+    <t>corsia (x)</t>
+  </si>
+  <si>
+    <t>corsia (y)</t>
+  </si>
+  <si>
+    <t>baseline (x)</t>
+  </si>
+  <si>
+    <t>baseline (y)</t>
   </si>
 </sst>
 </file>
@@ -3387,8 +3412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60248756-7A13-B544-A066-4CFE938C0EA1}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5105,6 +5130,875 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240D2AC3-9333-C244-8764-5B93F30ED127}">
+  <dimension ref="A1:H37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>672</v>
+      </c>
+      <c r="B1" t="s">
+        <v>673</v>
+      </c>
+      <c r="C1" t="s">
+        <v>674</v>
+      </c>
+      <c r="D1" t="s">
+        <v>675</v>
+      </c>
+      <c r="E1" t="s">
+        <v>676</v>
+      </c>
+      <c r="F1" t="s">
+        <v>677</v>
+      </c>
+      <c r="G1" t="s">
+        <v>678</v>
+      </c>
+      <c r="H1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2010.2642493997801</v>
+      </c>
+      <c r="B2">
+        <v>456.59680200789802</v>
+      </c>
+      <c r="C2">
+        <v>2012.9258356734199</v>
+      </c>
+      <c r="D2">
+        <v>516.42488843541605</v>
+      </c>
+      <c r="E2">
+        <v>2010.8551686656299</v>
+      </c>
+      <c r="F2">
+        <v>469.349926605429</v>
+      </c>
+      <c r="G2">
+        <v>2010.8551686656299</v>
+      </c>
+      <c r="H2">
+        <v>469.349926605429</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2011.4103379266801</v>
+      </c>
+      <c r="B3">
+        <v>485.56239764919502</v>
+      </c>
+      <c r="C3">
+        <v>2014.0204010801699</v>
+      </c>
+      <c r="D3">
+        <v>544.44005462721896</v>
+      </c>
+      <c r="E3">
+        <v>2011.9529900550799</v>
+      </c>
+      <c r="F3">
+        <v>493.16137823063201</v>
+      </c>
+      <c r="G3">
+        <v>2011.9529900550799</v>
+      </c>
+      <c r="H3">
+        <v>493.16137823063201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2012.50164379783</v>
+      </c>
+      <c r="B4">
+        <v>515.901056283755</v>
+      </c>
+      <c r="C4">
+        <v>2015.1180976533699</v>
+      </c>
+      <c r="D4">
+        <v>573.51417570658805</v>
+      </c>
+      <c r="E4">
+        <v>2013.05087924596</v>
+      </c>
+      <c r="F4">
+        <v>514.114095831349</v>
+      </c>
+      <c r="G4">
+        <v>2013.05087924596</v>
+      </c>
+      <c r="H4">
+        <v>514.114095831349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2013.59929876561</v>
+      </c>
+      <c r="B5">
+        <v>546.72940051451303</v>
+      </c>
+      <c r="C5">
+        <v>2016.17918046721</v>
+      </c>
+      <c r="D5">
+        <v>602.62574936779902</v>
+      </c>
+      <c r="E5">
+        <v>2014.14871373342</v>
+      </c>
+      <c r="F5">
+        <v>537.37329202000296</v>
+      </c>
+      <c r="G5">
+        <v>2014.14871373342</v>
+      </c>
+      <c r="H5">
+        <v>537.37329202000296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2014.6969337011501</v>
+      </c>
+      <c r="B6">
+        <v>578.40237070705098</v>
+      </c>
+      <c r="C6">
+        <v>2017.2402344434299</v>
+      </c>
+      <c r="D6">
+        <v>632.953213149813</v>
+      </c>
+      <c r="E6">
+        <v>2015.24654282759</v>
+      </c>
+      <c r="F6">
+        <v>560.85988750605998</v>
+      </c>
+      <c r="G6">
+        <v>2015.24654282759</v>
+      </c>
+      <c r="H6">
+        <v>560.85988750605998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2015.79455476822</v>
+      </c>
+      <c r="B7">
+        <v>610.66008195005202</v>
+      </c>
+      <c r="C7">
+        <v>2018.33785474003</v>
+      </c>
+      <c r="D7">
+        <v>665.24341000672996</v>
+      </c>
+      <c r="E7">
+        <v>2016.34438424928</v>
+      </c>
+      <c r="F7">
+        <v>583.82671316948199</v>
+      </c>
+      <c r="G7">
+        <v>2016.34438424928</v>
+      </c>
+      <c r="H7">
+        <v>583.82671316948199</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2016.8921627372799</v>
+      </c>
+      <c r="B8">
+        <v>643.47004862960102</v>
+      </c>
+      <c r="C8">
+        <v>2019.4354511520301</v>
+      </c>
+      <c r="D8">
+        <v>698.54066089499804</v>
+      </c>
+      <c r="E8">
+        <v>2017.44222567098</v>
+      </c>
+      <c r="F8">
+        <v>606.79353883290503</v>
+      </c>
+      <c r="G8">
+        <v>2017.44222567098</v>
+      </c>
+      <c r="H8">
+        <v>606.79353883290503</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2017.9897560674101</v>
+      </c>
+      <c r="B9">
+        <v>676.89724197352803</v>
+      </c>
+      <c r="C9">
+        <v>2020.53302907274</v>
+      </c>
+      <c r="D9">
+        <v>732.61756651721703</v>
+      </c>
+      <c r="E9">
+        <v>2018.5400678631399</v>
+      </c>
+      <c r="F9">
+        <v>629.72787888241396</v>
+      </c>
+      <c r="G9">
+        <v>2018.5400678631399</v>
+      </c>
+      <c r="H9">
+        <v>629.72787888241396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>2019.08732705388</v>
+      </c>
+      <c r="B10">
+        <v>711.26651812097896</v>
+      </c>
+      <c r="C10">
+        <v>2021.6122915759699</v>
+      </c>
+      <c r="D10">
+        <v>767.07318063972104</v>
+      </c>
+      <c r="E10">
+        <v>2019.6379285466101</v>
+      </c>
+      <c r="F10">
+        <v>651.88256419797096</v>
+      </c>
+      <c r="G10">
+        <v>2019.6379285466101</v>
+      </c>
+      <c r="H10">
+        <v>651.88256419797096</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>2020.18488417188</v>
+      </c>
+      <c r="B11">
+        <v>746.22053531889196</v>
+      </c>
+      <c r="C11">
+        <v>2022.6915343923399</v>
+      </c>
+      <c r="D11">
+        <v>802.35885820742203</v>
+      </c>
+      <c r="E11">
+        <v>2019.8886628077501</v>
+      </c>
+      <c r="F11">
+        <v>659.24614365530294</v>
+      </c>
+      <c r="G11">
+        <v>2019.8886628077501</v>
+      </c>
+      <c r="H11">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2021.28241663481</v>
+      </c>
+      <c r="B12">
+        <v>782.21409216207303</v>
+      </c>
+      <c r="C12">
+        <v>2023.7890483639801</v>
+      </c>
+      <c r="D12">
+        <v>839.13206978455298</v>
+      </c>
+      <c r="E12">
+        <v>2020.83451886178</v>
+      </c>
+      <c r="F12">
+        <v>678.80205261789797</v>
+      </c>
+      <c r="G12">
+        <v>2021.49476760121</v>
+      </c>
+      <c r="H12">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>2022.37992521315</v>
+      </c>
+      <c r="B13">
+        <v>819.21470303660703</v>
+      </c>
+      <c r="C13">
+        <v>2024.8865407624301</v>
+      </c>
+      <c r="D13">
+        <v>876.81487855129501</v>
+      </c>
+      <c r="E13">
+        <v>2021.52245601807</v>
+      </c>
+      <c r="F13">
+        <v>695.53803375829705</v>
+      </c>
+      <c r="G13">
+        <v>2022.5464060075201</v>
+      </c>
+      <c r="H13">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>2023.4591170721901</v>
+      </c>
+      <c r="B14">
+        <v>856.64891189700597</v>
+      </c>
+      <c r="C14">
+        <v>2025.9474328297399</v>
+      </c>
+      <c r="D14">
+        <v>913.96896205736505</v>
+      </c>
+      <c r="E14">
+        <v>2022.62022039269</v>
+      </c>
+      <c r="F14">
+        <v>721.75342081318104</v>
+      </c>
+      <c r="G14">
+        <v>2023.5980444138199</v>
+      </c>
+      <c r="H14">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>2024.50169322291</v>
+      </c>
+      <c r="B15">
+        <v>894.20274753996102</v>
+      </c>
+      <c r="C15">
+        <v>2026.9077059491101</v>
+      </c>
+      <c r="D15">
+        <v>948.321395347921</v>
+      </c>
+      <c r="E15">
+        <v>2023.7179716693099</v>
+      </c>
+      <c r="F15">
+        <v>748.52106330461299</v>
+      </c>
+      <c r="G15">
+        <v>2024.64968282012</v>
+      </c>
+      <c r="H15">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2025.52594351874</v>
+      </c>
+      <c r="B16">
+        <v>932.57536773376899</v>
+      </c>
+      <c r="C16">
+        <v>2027.8222438754899</v>
+      </c>
+      <c r="D16">
+        <v>981.37115569531397</v>
+      </c>
+      <c r="E16">
+        <v>2024.8157167821701</v>
+      </c>
+      <c r="F16">
+        <v>775.548590707362</v>
+      </c>
+      <c r="G16">
+        <v>2025.7013212264301</v>
+      </c>
+      <c r="H16">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2026.5135706952599</v>
+      </c>
+      <c r="B17">
+        <v>971.38008717076605</v>
+      </c>
+      <c r="C17">
+        <v>2028.7459068934299</v>
+      </c>
+      <c r="D17">
+        <v>1015.60681094837</v>
+      </c>
+      <c r="E17">
+        <v>2025.9134457151399</v>
+      </c>
+      <c r="F17">
+        <v>803.258316002318</v>
+      </c>
+      <c r="G17">
+        <v>2026.7529596327299</v>
+      </c>
+      <c r="H17">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2027.4279898709499</v>
+      </c>
+      <c r="B18">
+        <v>1009.4367726343399</v>
+      </c>
+      <c r="C18">
+        <v>2029.6878324899201</v>
+      </c>
+      <c r="D18">
+        <v>1051.6916235650999</v>
+      </c>
+      <c r="E18">
+        <v>2027.0111654024599</v>
+      </c>
+      <c r="F18">
+        <v>831.35786866424803</v>
+      </c>
+      <c r="G18">
+        <v>2027.80459803903</v>
+      </c>
+      <c r="H18">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2028.2234929654201</v>
+      </c>
+      <c r="B19">
+        <v>1044.2995937071901</v>
+      </c>
+      <c r="C19">
+        <v>2030.51332106167</v>
+      </c>
+      <c r="D19">
+        <v>1084.3627385935999</v>
+      </c>
+      <c r="E19">
+        <v>2028.10886428707</v>
+      </c>
+      <c r="F19">
+        <v>860.33453290187401</v>
+      </c>
+      <c r="G19">
+        <v>2028.8562364453401</v>
+      </c>
+      <c r="H19">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2028.99153943186</v>
+      </c>
+      <c r="B20">
+        <v>1079.03485885745</v>
+      </c>
+      <c r="C20">
+        <v>2031.32497632645</v>
+      </c>
+      <c r="D20">
+        <v>1118.2004711719201</v>
+      </c>
+      <c r="E20">
+        <v>2029.2065454508599</v>
+      </c>
+      <c r="F20">
+        <v>890.05836625953498</v>
+      </c>
+      <c r="G20">
+        <v>2029.9078748516399</v>
+      </c>
+      <c r="H20">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>2029.8052852539299</v>
+      </c>
+      <c r="B21">
+        <v>1116.5838191154401</v>
+      </c>
+      <c r="C21">
+        <v>2031.9020046782</v>
+      </c>
+      <c r="D21">
+        <v>1149.28707951507</v>
+      </c>
+      <c r="E21">
+        <v>2030.30419425487</v>
+      </c>
+      <c r="F21">
+        <v>921.14659540161006</v>
+      </c>
+      <c r="G21">
+        <v>2030.95951325794</v>
+      </c>
+      <c r="H21">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>2030.5458757403001</v>
+      </c>
+      <c r="B22">
+        <v>1151.16420782515</v>
+      </c>
+      <c r="C22">
+        <v>2032.6871155853401</v>
+      </c>
+      <c r="D22">
+        <v>1177.0151144517899</v>
+      </c>
+      <c r="E22">
+        <v>2031.4017860440499</v>
+      </c>
+      <c r="F22">
+        <v>954.63875997336595</v>
+      </c>
+      <c r="G22">
+        <v>2032.0111516642501</v>
+      </c>
+      <c r="H22">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2031.2772820963501</v>
+      </c>
+      <c r="B23">
+        <v>1187.04797277433</v>
+      </c>
+      <c r="C23">
+        <v>2033.4643031491701</v>
+      </c>
+      <c r="D23">
+        <v>1212.2614151535599</v>
+      </c>
+      <c r="E23">
+        <v>2032.4993084908699</v>
+      </c>
+      <c r="F23">
+        <v>991.05462979743697</v>
+      </c>
+      <c r="G23">
+        <v>2033.0627900705499</v>
+      </c>
+      <c r="H23">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>2031.99953777679</v>
+      </c>
+      <c r="B24">
+        <v>1222.8245516433999</v>
+      </c>
+      <c r="C24">
+        <v>2034.2506036433799</v>
+      </c>
+      <c r="D24">
+        <v>1249.2063665226401</v>
+      </c>
+      <c r="E24">
+        <v>2033.5419122982</v>
+      </c>
+      <c r="F24">
+        <v>1027.4423705914901</v>
+      </c>
+      <c r="G24">
+        <v>2034.11442847685</v>
+      </c>
+      <c r="H24">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2032.56635372711</v>
+      </c>
+      <c r="B25">
+        <v>1251.6453616388701</v>
+      </c>
+      <c r="C25">
+        <v>2035.0368801229199</v>
+      </c>
+      <c r="D25">
+        <v>1287.1638565072401</v>
+      </c>
+      <c r="E25">
+        <v>2034.5204624017299</v>
+      </c>
+      <c r="F25">
+        <v>1063.0365723653499</v>
+      </c>
+      <c r="G25">
+        <v>2035.1660668831601</v>
+      </c>
+      <c r="H25">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>2033.14230751893</v>
+      </c>
+      <c r="B26">
+        <v>1281.1144861908299</v>
+      </c>
+      <c r="C26">
+        <v>2035.7865603538</v>
+      </c>
+      <c r="D26">
+        <v>1324.4204896665301</v>
+      </c>
+      <c r="E26">
+        <v>2035.3983977590401</v>
+      </c>
+      <c r="F26">
+        <v>1095.6519655089701</v>
+      </c>
+      <c r="G26">
+        <v>2036.2177052894599</v>
+      </c>
+      <c r="H26">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>2033.8370774590401</v>
+      </c>
+      <c r="B27">
+        <v>1317.9909808260199</v>
+      </c>
+      <c r="C27">
+        <v>2036.4722179897501</v>
+      </c>
+      <c r="D27">
+        <v>1359.57192971425</v>
+      </c>
+      <c r="E27">
+        <v>2036.2671575285799</v>
+      </c>
+      <c r="F27">
+        <v>1129.2105524812</v>
+      </c>
+      <c r="G27">
+        <v>2037.26934369576</v>
+      </c>
+      <c r="H27">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>2034.45195595532</v>
+      </c>
+      <c r="B28">
+        <v>1351.5460756892101</v>
+      </c>
+      <c r="C28">
+        <v>2037.13956383645</v>
+      </c>
+      <c r="D28">
+        <v>1394.9491002468301</v>
+      </c>
+      <c r="E28">
+        <v>2037.11761010895</v>
+      </c>
+      <c r="F28">
+        <v>1162.80091492468</v>
+      </c>
+      <c r="G28">
+        <v>2038.32098210207</v>
+      </c>
+      <c r="H28">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2035.11684287657</v>
+      </c>
+      <c r="B29">
+        <v>1389.03916807059</v>
+      </c>
+      <c r="C29">
+        <v>2037.8343147242899</v>
+      </c>
+      <c r="D29">
+        <v>1432.62890201502</v>
+      </c>
+      <c r="E29">
+        <v>2037.9314589678099</v>
+      </c>
+      <c r="F29">
+        <v>1196.00550056308</v>
+      </c>
+      <c r="G29">
+        <v>2039.3726205083699</v>
+      </c>
+      <c r="H29">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>2036.30511005433</v>
+      </c>
+      <c r="B30">
+        <v>1458.65641841044</v>
+      </c>
+      <c r="C30">
+        <v>2038.5107511851199</v>
+      </c>
+      <c r="D30">
+        <v>1470.6456506806201</v>
+      </c>
+      <c r="E30">
+        <v>2038.8092938228999</v>
+      </c>
+      <c r="F30">
+        <v>1232.85840256914</v>
+      </c>
+      <c r="G30">
+        <v>2040.42425891467</v>
+      </c>
+      <c r="H30">
+        <v>659.24614365530294</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>2036.8352198555599</v>
+      </c>
+      <c r="B31">
+        <v>1491.4101398867001</v>
+      </c>
+      <c r="C31">
+        <v>2039.15059275148</v>
+      </c>
+      <c r="D31">
+        <v>1507.9044452872599</v>
+      </c>
+      <c r="E31">
+        <v>2039.62308731592</v>
+      </c>
+      <c r="F31">
+        <v>1268.3973965001301</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2037.2647733654201</v>
+      </c>
+      <c r="B32">
+        <v>1518.72040146731</v>
+      </c>
+      <c r="C32">
+        <v>2039.7172927443701</v>
+      </c>
+      <c r="D32">
+        <v>1541.6144066740401</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2037.6943088882899</v>
+      </c>
+      <c r="B33">
+        <v>1546.7890544709401</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2038.1969233070799</v>
+      </c>
+      <c r="B34">
+        <v>1581.0492350459101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2038.72691867039</v>
+      </c>
+      <c r="B35">
+        <v>1618.62804053799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2039.2203101719299</v>
+      </c>
+      <c r="B36">
+        <v>1655.82698341779</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2039.6770923337299</v>
+      </c>
+      <c r="B37">
+        <v>1692.8770328303799</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8018BEA-49B9-1B42-9A7A-5348ADC7F270}">
   <dimension ref="A1:L28"/>
   <sheetViews>
@@ -5773,7 +6667,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C5AF1E-8720-AD4D-AE69-58E15F872AB8}">
   <dimension ref="A1:T12"/>
   <sheetViews>

</xml_diff>